<commit_message>
Sửa lỗi giao diện + thêm link báo lỗi
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/links.xlsx
+++ b/Hethongquanlylab/wwwroot/data/links.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EF5662-AD71-41AC-AB07-CA5E7C2F2BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0D8C2F-1BB9-4C23-9D0D-9EA201E2411C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Link</t>
   </si>
@@ -33,24 +33,37 @@
     <t>Biểu mẫu</t>
   </si>
   <si>
-    <t>https://www.youtube.com/</t>
+    <t>https://www.youtube.com/1</t>
   </si>
   <si>
     <t>Lịch làm việc</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=gFIUxGJHXRk</t>
+    <t>https://www.youtube.com/watch?v=gFIUxGJHXRk2</t>
+  </si>
+  <si>
+    <t>Báo lỗi</t>
+  </si>
+  <si>
+    <t>https://husteduvn-my.sharepoint.com/:x:/g/personal/hinh_nx204650_sis_hust_edu_vn/EX9vkOmM92xJsgH0WFu1WNQBAF8wYkouriFIwiYqTkbdvQ?e=ijYfty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -73,13 +86,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -358,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -370,29 +386,39 @@
     <col min="2" max="2" width="71.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>